<commit_message>
finish tests of lab26
</commit_message>
<xml_diff>
--- a/lab25/lab25/sort test.xlsx
+++ b/lab25/lab25/sort test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Сводная" sheetId="4" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>AMD Ryzen 5 5600 4650 MHz singlecore | 4450 MHz multicore</t>
   </si>
   <si>
-    <t>16,0 ГБ 3600 MT/s</t>
-  </si>
-  <si>
     <t>WDC  WDS500G2B0A-00SM50 500,1 GB</t>
   </si>
   <si>
@@ -436,6 +433,9 @@
   </si>
   <si>
     <t>0.0056000000</t>
+  </si>
+  <si>
+    <t>32 ГБ 3600 MT/s 2  двухранковых планки</t>
   </si>
 </sst>
 </file>
@@ -886,7 +886,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -946,15 +946,15 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:3">
@@ -967,7 +967,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:3">
@@ -975,7 +975,7 @@
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:3">
@@ -996,7 +996,7 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:3">
@@ -1006,7 +1006,7 @@
     </row>
     <row r="20" spans="2:3">
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="2:3">
@@ -1016,12 +1016,12 @@
     </row>
     <row r="24" spans="2:3">
       <c r="C24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="C25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="2:3">
@@ -1071,19 +1071,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1091,19 +1091,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1111,19 +1111,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1131,19 +1131,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1151,39 +1151,39 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.2" customHeight="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1228,19 +1228,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1248,19 +1248,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1268,19 +1268,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1288,19 +1288,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1308,39 +1308,39 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1352,7 +1352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1385,19 +1385,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1">
@@ -1405,19 +1405,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1425,19 +1425,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1445,19 +1445,19 @@
         <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" thickBot="1">
@@ -1465,39 +1465,39 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>